<commit_message>
add support for institution import
</commit_message>
<xml_diff>
--- a/public/example.xlsx
+++ b/public/example.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elisj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE20C270-FCD0-481B-BF5B-FD657F1C7639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F217D746-96C9-4C65-8CE7-10E300C71DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F80E1CF5-67E3-4239-A4DF-3A660E92E80C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F80E1CF5-67E3-4239-A4DF-3A660E92E80C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="העברות" sheetId="1" r:id="rId1"/>
+    <sheet name="מוסד" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>תעודת זהות</t>
   </si>
@@ -58,6 +59,24 @@
   </si>
   <si>
     <t>טסט טסט</t>
+  </si>
+  <si>
+    <t>מזהה מוסד</t>
+  </si>
+  <si>
+    <t>מזהה מוסד שולח</t>
+  </si>
+  <si>
+    <t>שם מוסד</t>
+  </si>
+  <si>
+    <t>מספר מזהה</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>החברה שלי בע"מ</t>
   </si>
 </sst>
 </file>
@@ -93,8 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,12 +432,16 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>18</v>
       </c>
@@ -466,4 +490,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6704F40B-C909-4289-9D59-E93F318E7AF1}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>12345678</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add support for institution import (#1)
</commit_message>
<xml_diff>
--- a/public/example.xlsx
+++ b/public/example.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elisj\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE20C270-FCD0-481B-BF5B-FD657F1C7639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F217D746-96C9-4C65-8CE7-10E300C71DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F80E1CF5-67E3-4239-A4DF-3A660E92E80C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F80E1CF5-67E3-4239-A4DF-3A660E92E80C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="העברות" sheetId="1" r:id="rId1"/>
+    <sheet name="מוסד" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>תעודת זהות</t>
   </si>
@@ -58,6 +59,24 @@
   </si>
   <si>
     <t>טסט טסט</t>
+  </si>
+  <si>
+    <t>מזהה מוסד</t>
+  </si>
+  <si>
+    <t>מזהה מוסד שולח</t>
+  </si>
+  <si>
+    <t>שם מוסד</t>
+  </si>
+  <si>
+    <t>מספר מזהה</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>החברה שלי בע"מ</t>
   </si>
 </sst>
 </file>
@@ -93,8 +112,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,12 +432,16 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>18</v>
       </c>
@@ -466,4 +490,54 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6704F40B-C909-4289-9D59-E93F318E7AF1}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.77734375" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>12345678</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>